<commit_message>
Updated excel sheet with exact EPS specs. Sent out requests for quotes to 13 suppliers. Added CAD model.
</commit_message>
<xml_diff>
--- a/excelWorkbook/Material_Cost_Source.xlsx
+++ b/excelWorkbook/Material_Cost_Source.xlsx
@@ -15,18 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
   <si>
     <t>Material</t>
   </si>
   <si>
-    <t>Length (Feet)</t>
-  </si>
-  <si>
-    <t>Width (Feet)</t>
-  </si>
-  <si>
-    <t>Height (Feet)</t>
+    <t>Length (Inches)</t>
+  </si>
+  <si>
+    <t>Width (Inches)</t>
+  </si>
+  <si>
+    <t>Depth (Inches)</t>
   </si>
   <si>
     <t>Length (mm)</t>
@@ -35,7 +35,7 @@
     <t>Width (mm)</t>
   </si>
   <si>
-    <t>Height (mm)</t>
+    <t>Depth (mm)</t>
   </si>
   <si>
     <t>Cost</t>
@@ -47,13 +47,85 @@
     <t>Source</t>
   </si>
   <si>
+    <t>Location</t>
+  </si>
+  <si>
     <t>EPS Foam</t>
   </si>
   <si>
-    <t>google.com</t>
+    <t>North Air Plenum Back &amp; Front</t>
+  </si>
+  <si>
+    <t>North Air Plenum Mid Shelf</t>
+  </si>
+  <si>
+    <t>North Air Plenum Shelf Support</t>
+  </si>
+  <si>
+    <t>North Air Plenum Ends</t>
+  </si>
+  <si>
+    <t>North Air Plenum Bottom</t>
+  </si>
+  <si>
+    <t>North Air Plenum Top</t>
+  </si>
+  <si>
+    <t>Thermal Battery Walls</t>
+  </si>
+  <si>
+    <t>South Plenum Front &amp; Back</t>
+  </si>
+  <si>
+    <t>South Plenumm Ends</t>
+  </si>
+  <si>
+    <t>South Plenum Top</t>
+  </si>
+  <si>
+    <t>Side Foundation</t>
+  </si>
+  <si>
+    <t>End Foundation</t>
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Front and Back</t>
+  </si>
+  <si>
+    <t>North Insulation Ends</t>
+  </si>
+  <si>
+    <t>North Insulation Middle</t>
+  </si>
+  <si>
+    <t>North Insulation Base Ends</t>
+  </si>
+  <si>
+    <t>North Insulation Base Middle</t>
+  </si>
+  <si>
+    <t>North Insulation Triangle Ends</t>
+  </si>
+  <si>
+    <t>North Insulation Triangle Middle</t>
+  </si>
+  <si>
+    <t>North Insulation Air Intake Ends</t>
+  </si>
+  <si>
+    <t>North Insulation Air Intake Middle</t>
+  </si>
+  <si>
+    <t>Air Intake</t>
+  </si>
+  <si>
+    <t>South PVC Anchor Ends</t>
+  </si>
+  <si>
+    <t>South PVC Anchor Middle</t>
   </si>
 </sst>
 </file>
@@ -398,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,44 +507,431 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>59.14</v>
+      </c>
+      <c r="C2">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1502.156</v>
+      </c>
+      <c r="F2">
+        <v>660.4</v>
+      </c>
+      <c r="G2">
+        <v>25.4</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>96</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2438.4</v>
+      </c>
+      <c r="F3">
+        <v>558.8</v>
+      </c>
+      <c r="G3">
+        <v>25.4</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>558.8</v>
+      </c>
+      <c r="F4">
+        <v>431.8</v>
+      </c>
+      <c r="G4">
+        <v>25.4</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>660.4</v>
+      </c>
+      <c r="F5">
+        <v>558.8</v>
+      </c>
+      <c r="G5">
+        <v>25.4</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>93.64</v>
+      </c>
+      <c r="C6">
+        <v>23.906</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2378.456</v>
+      </c>
+      <c r="F6">
+        <v>607.2123999999999</v>
+      </c>
+      <c r="G6">
+        <v>50.8</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>53.14</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1349.756</v>
+      </c>
+      <c r="F7">
+        <v>609.5999999999999</v>
+      </c>
+      <c r="G7">
+        <v>50.8</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>96</v>
+      </c>
+      <c r="C8">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>2438.4</v>
+      </c>
+      <c r="F8">
+        <v>1219.2</v>
+      </c>
+      <c r="G8">
+        <v>152.4</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>68</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1727.2</v>
+      </c>
+      <c r="F9">
+        <v>558.8</v>
+      </c>
+      <c r="G9">
+        <v>50.8</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>23.906</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>558.8</v>
+      </c>
+      <c r="F10">
+        <v>607.2123999999999</v>
+      </c>
+      <c r="G10">
+        <v>50.8</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>72</v>
+      </c>
+      <c r="C11">
+        <v>23.906</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>1828.8</v>
+      </c>
+      <c r="F11">
+        <v>607.2123999999999</v>
+      </c>
+      <c r="G11">
+        <v>50.8</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>96</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2438.4</v>
+      </c>
+      <c r="F12">
+        <v>304.8</v>
+      </c>
+      <c r="G12">
+        <v>101.6</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>10</v>
       </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
+      <c r="K12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>96</v>
+      </c>
+      <c r="C13">
+        <v>36</v>
+      </c>
+      <c r="D13">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>0.5</v>
-      </c>
-      <c r="E2">
+      <c r="E13">
         <v>2438.4</v>
       </c>
-      <c r="F2">
-        <v>1219.2</v>
-      </c>
-      <c r="G2">
-        <v>152.4</v>
-      </c>
-      <c r="H2">
-        <v>12.9</v>
-      </c>
-      <c r="I2">
-        <v>68</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="F13">
+        <v>914.4</v>
+      </c>
+      <c r="G13">
+        <v>101.6</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>914.4</v>
+      </c>
+      <c r="F14">
+        <v>914.4</v>
+      </c>
+      <c r="G14">
+        <v>101.6</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
         <f>SUM(B2:B5)</f>
         <v>0</v>
       </c>
@@ -484,13 +943,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,101 +980,488 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>2438.4</v>
       </c>
       <c r="F2">
-        <v>609.6</v>
+        <v>1219.2</v>
       </c>
       <c r="G2">
         <v>152.4</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>0.1666666666666667</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>2438.4</v>
+        <v>1803.4</v>
       </c>
       <c r="F3">
-        <v>1219.2</v>
+        <v>1066.8</v>
       </c>
       <c r="G3">
         <v>50.8</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>90</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>71</v>
+      </c>
+      <c r="C4">
+        <v>48</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1803.4</v>
+      </c>
+      <c r="F4">
+        <v>1219.2</v>
+      </c>
+      <c r="G4">
+        <v>50.8</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>27.8</v>
+      </c>
+      <c r="C5">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>706.12</v>
+      </c>
+      <c r="F5">
+        <v>1066.8</v>
+      </c>
+      <c r="G5">
+        <v>152.4</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>27.8</v>
+      </c>
+      <c r="C6">
+        <v>48</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>706.12</v>
+      </c>
+      <c r="F6">
+        <v>1219.2</v>
+      </c>
+      <c r="G6">
+        <v>152.4</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>48.625</v>
+      </c>
+      <c r="C7">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1235.075</v>
+      </c>
+      <c r="F7">
+        <v>1066.8</v>
+      </c>
+      <c r="G7">
+        <v>50.8</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>48.625</v>
+      </c>
+      <c r="C8">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1235.075</v>
+      </c>
+      <c r="F8">
+        <v>1219.2</v>
+      </c>
+      <c r="G8">
+        <v>50.8</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>15.6875</v>
+      </c>
+      <c r="C9">
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>398.4625</v>
+      </c>
+      <c r="F9">
+        <v>1066.8</v>
+      </c>
+      <c r="G9">
+        <v>50.8</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>15.6875</v>
+      </c>
+      <c r="C10">
+        <v>48</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>398.4625</v>
+      </c>
+      <c r="F10">
+        <v>1219.2</v>
+      </c>
+      <c r="G10">
+        <v>50.8</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>10.7656</v>
+      </c>
+      <c r="C11">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>273.44624</v>
+      </c>
+      <c r="F11">
+        <v>1066.8</v>
+      </c>
+      <c r="G11">
+        <v>50.8</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>10.7656</v>
+      </c>
+      <c r="C12">
+        <v>48</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>273.44624</v>
+      </c>
+      <c r="F12">
+        <v>1219.2</v>
+      </c>
+      <c r="G12">
+        <v>50.8</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="K12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>60.28</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1531.112</v>
+      </c>
+      <c r="F13">
+        <v>609.5999999999999</v>
+      </c>
+      <c r="G13">
+        <v>50.8</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>60.28</v>
+      </c>
+      <c r="C14">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>1531.112</v>
+      </c>
+      <c r="F14">
+        <v>558.8</v>
+      </c>
+      <c r="G14">
+        <v>50.8</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>42</v>
+      </c>
+      <c r="C15">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>2.166666666666667</v>
-      </c>
-      <c r="D4">
-        <v>0.08333333333333333</v>
-      </c>
-      <c r="E4">
-        <v>2438.4</v>
-      </c>
-      <c r="F4">
-        <v>660.4</v>
-      </c>
-      <c r="G4">
-        <v>25.4</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>1066.8</v>
+      </c>
+      <c r="F15">
+        <v>254</v>
+      </c>
+      <c r="G15">
+        <v>152.4</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>48</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>1219.2</v>
+      </c>
+      <c r="F16">
+        <v>254</v>
+      </c>
+      <c r="G16">
+        <v>152.4</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="K16" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Posting update getting close to putting the big lego set together
</commit_message>
<xml_diff>
--- a/excelWorkbook/Material_Cost_Source.xlsx
+++ b/excelWorkbook/Material_Cost_Source.xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Thermal Battery" sheetId="1" r:id="rId1"/>
+    <sheet name="Greenhouse" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
   <si>
     <t>Material</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>South PVC Anchor Middle</t>
+  </si>
+  <si>
+    <t>Item</t>
   </si>
 </sst>
 </file>
@@ -943,7 +946,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1464,6 +1467,11 @@
         <v>36</v>
       </c>
     </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>